<commit_message>
modified:   NC Signups.xlsx 	modified:   Tools and Guidelines.docx
</commit_message>
<xml_diff>
--- a/NC Signups.xlsx
+++ b/NC Signups.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Sachin Doolarchan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bryanjangeesingh@gmail.com </t>
+  </si>
+  <si>
+    <t>gtatrinidad@hotmail.com</t>
+  </si>
+  <si>
+    <t>jared.hamid@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -479,7 +488,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,6 +520,9 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -522,6 +534,9 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -623,6 +638,9 @@
       </c>
       <c r="C12" t="s">
         <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,6 +746,9 @@
     <hyperlink ref="E15" r:id="rId2"/>
     <hyperlink ref="E5" r:id="rId3"/>
     <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E12" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new file:   Event/22nd February Plan of action.docx 	new file:   Event/Event.xlsx 	modified:   NC Signups.xlsx 	new file:   NGHS Signups.xlsx 	new file:   New Microsoft Word Document.docx 	new file:   ~$ols and Guidelines.docx 	new file:   ~$w Microsoft Word Document.docx
</commit_message>
<xml_diff>
--- a/NC Signups.xlsx
+++ b/NC Signups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>jared.hamid@gmail.com</t>
+  </si>
+  <si>
+    <t>Amar Harripersad</t>
+  </si>
+  <si>
+    <t>amarharr@gmail.com</t>
+  </si>
+  <si>
+    <t>6BS1</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>756-7332</t>
+  </si>
+  <si>
+    <t>Sean-Michael Gopaul</t>
   </si>
 </sst>
 </file>
@@ -485,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,7 +517,8 @@
     <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -509,6 +531,12 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -520,7 +548,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -534,7 +562,7 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -559,7 +587,7 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -639,7 +667,7 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -653,7 +681,7 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -667,8 +695,11 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,7 +712,7 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -696,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -707,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -718,7 +749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -729,7 +760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -740,15 +771,44 @@
         <v>5</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>7046465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1"/>
-    <hyperlink ref="E15" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="E12" r:id="rId5"/>
-    <hyperlink ref="E3" r:id="rId6"/>
-    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId1"/>
+    <hyperlink ref="D15" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D13" r:id="rId4"/>
+    <hyperlink ref="D12" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId7"/>
+    <hyperlink ref="D21" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NC Signups.xlsx 	modified:   NGHS Signups.xlsx
</commit_message>
<xml_diff>
--- a/NC Signups.xlsx
+++ b/NC Signups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Sean-Michael Gopaul</t>
+  </si>
+  <si>
+    <t>Anirudh Madala</t>
+  </si>
+  <si>
+    <t>787-4565</t>
+  </si>
+  <si>
+    <t>qertyblue@gmail.com</t>
+  </si>
+  <si>
+    <t>704-6465</t>
+  </si>
+  <si>
+    <t>738-3113</t>
   </si>
 </sst>
 </file>
@@ -506,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,8 +799,8 @@
       <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E21">
-        <v>7046465</v>
+      <c r="E21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -797,6 +812,26 @@
       </c>
       <c r="C22" t="s">
         <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -809,6 +844,7 @@
     <hyperlink ref="D3" r:id="rId6"/>
     <hyperlink ref="D2" r:id="rId7"/>
     <hyperlink ref="D21" r:id="rId8"/>
+    <hyperlink ref="D22" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>